<commit_message>
add check forecast counter
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80000571.xlsx
+++ b/eq_log/eq_file/80000571.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -131,6 +131,33 @@
   </si>
   <si>
     <t>34</t>
+  </si>
+  <si>
+    <t>13/02/2018</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>319993</t>
+  </si>
+  <si>
+    <t>320000</t>
+  </si>
+  <si>
+    <t>639999</t>
   </si>
   <si>
     <t>**</t>
@@ -1253,6 +1280,15 @@
       <c r="A29" t="s">
         <v>39</v>
       </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
       <c r="E29" s="19">
         <f>D29-D28</f>
         <v/>
@@ -1263,6 +1299,18 @@
       </c>
     </row>
     <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
       <c r="E30" s="19">
         <f>D30-D29</f>
         <v/>
@@ -1273,6 +1321,18 @@
       </c>
     </row>
     <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
       <c r="E31" s="19">
         <f>D31-D30</f>
         <v/>
@@ -1283,6 +1343,18 @@
       </c>
     </row>
     <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
       <c r="E32" s="19">
         <f>D32-D31</f>
         <v/>
@@ -1293,6 +1365,18 @@
       </c>
     </row>
     <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
       <c r="E33" s="19">
         <f>D33-D32</f>
         <v/>
@@ -1303,6 +1387,18 @@
       </c>
     </row>
     <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
       <c r="E34" s="19">
         <f>D34-D33</f>
         <v/>
@@ -1313,6 +1409,18 @@
       </c>
     </row>
     <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>46</v>
+      </c>
       <c r="E35" s="19">
         <f>D35-D34</f>
         <v/>
@@ -1323,6 +1431,18 @@
       </c>
     </row>
     <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
       <c r="E36" s="19">
         <f>D36-D35</f>
         <v/>
@@ -1333,6 +1453,9 @@
       </c>
     </row>
     <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
       <c r="E37" s="19">
         <f>D37-D36</f>
         <v/>

</xml_diff>

<commit_message>
add 2 spare parts, need decision without second spare parts
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80000571.xlsx
+++ b/eq_log/eq_file/80000571.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>22/02/2018</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>**</t>
@@ -1612,6 +1621,15 @@
       <c r="A43" t="s">
         <v>56</v>
       </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
       <c r="E43" s="19">
         <f>D43-D42</f>
         <v/>
@@ -1622,6 +1640,18 @@
       </c>
     </row>
     <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" t="s">
+        <v>58</v>
+      </c>
       <c r="E44" s="19">
         <f>D44-D43</f>
         <v/>
@@ -1632,6 +1662,9 @@
       </c>
     </row>
     <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
       <c r="E45" s="19">
         <f>D45-D44</f>
         <v/>

</xml_diff>

<commit_message>
same refactoring, second spare parts is not working
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80000571.xlsx
+++ b/eq_log/eq_file/80000571.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -191,6 +191,36 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>3070</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>3067</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
   <si>
     <t>**</t>
@@ -1663,7 +1693,16 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" t="s">
         <v>59</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
       </c>
       <c r="E45" s="19">
         <f>D45-D44</f>
@@ -1675,6 +1714,18 @@
       </c>
     </row>
     <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>61</v>
+      </c>
       <c r="E46" s="19">
         <f>D46-D45</f>
         <v/>
@@ -1685,6 +1736,18 @@
       </c>
     </row>
     <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
+        <v>62</v>
+      </c>
       <c r="E47" s="19">
         <f>D47-D46</f>
         <v/>
@@ -1695,6 +1758,18 @@
       </c>
     </row>
     <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
       <c r="E48" s="19">
         <f>D48-D47</f>
         <v/>
@@ -1705,6 +1780,18 @@
       </c>
     </row>
     <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" t="s">
+        <v>64</v>
+      </c>
       <c r="E49" s="19">
         <f>D49-D48</f>
         <v/>
@@ -1715,6 +1802,18 @@
       </c>
     </row>
     <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
       <c r="E50" s="19">
         <f>D50-D49</f>
         <v/>
@@ -1725,6 +1824,18 @@
       </c>
     </row>
     <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
       <c r="E51" s="19">
         <f>D51-D50</f>
         <v/>
@@ -1735,6 +1846,18 @@
       </c>
     </row>
     <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" t="s">
+        <v>21</v>
+      </c>
       <c r="E52" s="19">
         <f>D52-D51</f>
         <v/>
@@ -1745,6 +1868,18 @@
       </c>
     </row>
     <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
       <c r="E53" s="19">
         <f>D53-D52</f>
         <v/>
@@ -1755,6 +1890,18 @@
       </c>
     </row>
     <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" t="s">
+        <v>66</v>
+      </c>
       <c r="E54" s="19">
         <f>D54-D53</f>
         <v/>
@@ -1765,6 +1912,18 @@
       </c>
     </row>
     <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" t="s">
+        <v>67</v>
+      </c>
       <c r="E55" s="19">
         <f>D55-D54</f>
         <v/>
@@ -1775,6 +1934,18 @@
       </c>
     </row>
     <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" t="s">
+        <v>68</v>
+      </c>
       <c r="E56" s="19">
         <f>D56-D55</f>
         <v/>
@@ -1785,6 +1956,9 @@
       </c>
     </row>
     <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
       <c r="E57" s="19">
         <f>D57-D56</f>
         <v/>

</xml_diff>

<commit_message>
add with mistake spare parts to log file
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80000571.xlsx
+++ b/eq_log/eq_file/80000571.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -221,6 +221,99 @@
   </si>
   <si>
     <t>18</t>
+  </si>
+  <si>
+    <t>27/02/2018</t>
+  </si>
+  <si>
+    <t>04/03/2018</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>227</t>
+  </si>
+  <si>
+    <t>228</t>
+  </si>
+  <si>
+    <t>229</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>236</t>
+  </si>
+  <si>
+    <t>237</t>
+  </si>
+  <si>
+    <t>Не симетричне / не відповідне закриття ядра</t>
+  </si>
+  <si>
+    <t>238</t>
+  </si>
+  <si>
+    <t>239</t>
+  </si>
+  <si>
+    <t>05/03/2018</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>242</t>
+  </si>
+  <si>
+    <t>243</t>
+  </si>
+  <si>
+    <t>244</t>
   </si>
   <si>
     <t>**</t>
@@ -1959,6 +2052,15 @@
       <c r="A57" t="s">
         <v>69</v>
       </c>
+      <c r="B57" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" t="s">
+        <v>23</v>
+      </c>
       <c r="E57" s="19">
         <f>D57-D56</f>
         <v/>
@@ -1969,6 +2071,18 @@
       </c>
     </row>
     <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" t="s">
+        <v>24</v>
+      </c>
       <c r="E58" s="19">
         <f>D58-D57</f>
         <v/>
@@ -1979,6 +2093,18 @@
       </c>
     </row>
     <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
+      </c>
       <c r="E59" s="19">
         <f>D59-D58</f>
         <v/>
@@ -1989,6 +2115,18 @@
       </c>
     </row>
     <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" t="s">
+        <v>71</v>
+      </c>
       <c r="E60" s="19">
         <f>D60-D59</f>
         <v/>
@@ -1999,6 +2137,18 @@
       </c>
     </row>
     <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
       <c r="E61" s="19">
         <f>D61-D60</f>
         <v/>
@@ -2009,6 +2159,18 @@
       </c>
     </row>
     <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" t="s">
+        <v>73</v>
+      </c>
       <c r="E62" s="19">
         <f>D62-D61</f>
         <v/>
@@ -2019,6 +2181,18 @@
       </c>
     </row>
     <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" t="s">
+        <v>71</v>
+      </c>
       <c r="E63" s="19">
         <f>D63-D62</f>
         <v/>
@@ -2029,6 +2203,18 @@
       </c>
     </row>
     <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" t="s">
+        <v>74</v>
+      </c>
       <c r="E64" s="19">
         <f>D64-D63</f>
         <v/>
@@ -2039,6 +2225,18 @@
       </c>
     </row>
     <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" t="s">
+        <v>59</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" t="s">
+        <v>74</v>
+      </c>
       <c r="E65" s="19">
         <f>D65-D64</f>
         <v/>
@@ -2049,6 +2247,18 @@
       </c>
     </row>
     <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" t="s">
+        <v>71</v>
+      </c>
       <c r="E66" s="19">
         <f>D66-D65</f>
         <v/>
@@ -2059,6 +2269,18 @@
       </c>
     </row>
     <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" t="s">
+        <v>72</v>
+      </c>
       <c r="E67" s="19">
         <f>D67-D66</f>
         <v/>
@@ -2069,6 +2291,18 @@
       </c>
     </row>
     <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>73</v>
+      </c>
       <c r="E68" s="19">
         <f>D68-D67</f>
         <v/>
@@ -2079,6 +2313,18 @@
       </c>
     </row>
     <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" t="s">
+        <v>75</v>
+      </c>
       <c r="E69" s="19">
         <f>D69-D68</f>
         <v/>
@@ -2089,6 +2335,18 @@
       </c>
     </row>
     <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" t="s">
+        <v>27</v>
+      </c>
       <c r="E70" s="19">
         <f>D70-D69</f>
         <v/>
@@ -2099,6 +2357,18 @@
       </c>
     </row>
     <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>59</v>
+      </c>
+      <c r="C71" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
       <c r="E71" s="19">
         <f>D71-D70</f>
         <v/>
@@ -2109,6 +2379,18 @@
       </c>
     </row>
     <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" t="s">
+        <v>29</v>
+      </c>
       <c r="E72" s="19">
         <f>D72-D71</f>
         <v/>
@@ -2119,6 +2401,18 @@
       </c>
     </row>
     <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" t="s">
+        <v>59</v>
+      </c>
+      <c r="C73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" t="s">
+        <v>30</v>
+      </c>
       <c r="E73" s="19">
         <f>D73-D72</f>
         <v/>
@@ -2129,6 +2423,18 @@
       </c>
     </row>
     <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" t="s">
+        <v>31</v>
+      </c>
       <c r="E74" s="19">
         <f>D74-D73</f>
         <v/>
@@ -2139,6 +2445,18 @@
       </c>
     </row>
     <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" t="s">
+        <v>33</v>
+      </c>
       <c r="E75" s="19">
         <f>D75-D74</f>
         <v/>
@@ -2149,6 +2467,18 @@
       </c>
     </row>
     <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" t="s">
+        <v>35</v>
+      </c>
       <c r="E76" s="19">
         <f>D76-D75</f>
         <v/>
@@ -2159,6 +2489,18 @@
       </c>
     </row>
     <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>70</v>
+      </c>
+      <c r="B77" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77" t="s">
+        <v>37</v>
+      </c>
       <c r="E77" s="19">
         <f>D77-D76</f>
         <v/>
@@ -2169,6 +2511,18 @@
       </c>
     </row>
     <row r="78" spans="1:8">
+      <c r="A78" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>38</v>
+      </c>
       <c r="E78" s="19">
         <f>D78-D77</f>
         <v/>
@@ -2179,6 +2533,18 @@
       </c>
     </row>
     <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" t="s">
+        <v>26</v>
+      </c>
+      <c r="D79" t="s">
+        <v>76</v>
+      </c>
       <c r="E79" s="19">
         <f>D79-D78</f>
         <v/>
@@ -2189,6 +2555,18 @@
       </c>
     </row>
     <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" t="s">
+        <v>77</v>
+      </c>
       <c r="E80" s="19">
         <f>D80-D79</f>
         <v/>
@@ -2199,6 +2577,18 @@
       </c>
     </row>
     <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>70</v>
+      </c>
+      <c r="B81" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" t="s">
+        <v>26</v>
+      </c>
+      <c r="D81" t="s">
+        <v>78</v>
+      </c>
       <c r="E81" s="19">
         <f>D81-D80</f>
         <v/>
@@ -2209,6 +2599,18 @@
       </c>
     </row>
     <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" t="s">
+        <v>59</v>
+      </c>
+      <c r="C82" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" t="s">
+        <v>79</v>
+      </c>
       <c r="E82" s="19">
         <f>D82-D81</f>
         <v/>
@@ -2219,6 +2621,18 @@
       </c>
     </row>
     <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>70</v>
+      </c>
+      <c r="B83" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D83" t="s">
+        <v>80</v>
+      </c>
       <c r="E83" s="19">
         <f>D83-D82</f>
         <v/>
@@ -2229,6 +2643,18 @@
       </c>
     </row>
     <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84" t="s">
+        <v>59</v>
+      </c>
+      <c r="C84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" t="s">
+        <v>81</v>
+      </c>
       <c r="E84" s="19">
         <f>D84-D83</f>
         <v/>
@@ -2239,6 +2665,18 @@
       </c>
     </row>
     <row r="85" spans="1:8">
+      <c r="A85" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" t="s">
+        <v>82</v>
+      </c>
       <c r="E85" s="19">
         <f>D85-D84</f>
         <v/>
@@ -2249,6 +2687,18 @@
       </c>
     </row>
     <row r="86" spans="1:8">
+      <c r="A86" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" t="s">
+        <v>59</v>
+      </c>
+      <c r="C86" t="s">
+        <v>26</v>
+      </c>
+      <c r="D86" t="s">
+        <v>83</v>
+      </c>
       <c r="E86" s="19">
         <f>D86-D85</f>
         <v/>
@@ -2259,6 +2709,18 @@
       </c>
     </row>
     <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" t="s">
+        <v>59</v>
+      </c>
+      <c r="C87" t="s">
+        <v>26</v>
+      </c>
+      <c r="D87" t="s">
+        <v>84</v>
+      </c>
       <c r="E87" s="19">
         <f>D87-D86</f>
         <v/>
@@ -2269,6 +2731,18 @@
       </c>
     </row>
     <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88" t="s">
+        <v>59</v>
+      </c>
+      <c r="C88" t="s">
+        <v>26</v>
+      </c>
+      <c r="D88" t="s">
+        <v>85</v>
+      </c>
       <c r="E88" s="19">
         <f>D88-D87</f>
         <v/>
@@ -2279,6 +2753,18 @@
       </c>
     </row>
     <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>70</v>
+      </c>
+      <c r="B89" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D89" t="s">
+        <v>86</v>
+      </c>
       <c r="E89" s="19">
         <f>D89-D88</f>
         <v/>
@@ -2289,6 +2775,18 @@
       </c>
     </row>
     <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90" t="s">
+        <v>59</v>
+      </c>
+      <c r="C90" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" t="s">
+        <v>87</v>
+      </c>
       <c r="E90" s="19">
         <f>D90-D89</f>
         <v/>
@@ -2299,6 +2797,18 @@
       </c>
     </row>
     <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>70</v>
+      </c>
+      <c r="B91" t="s">
+        <v>59</v>
+      </c>
+      <c r="C91" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" t="s">
+        <v>88</v>
+      </c>
       <c r="E91" s="19">
         <f>D91-D90</f>
         <v/>
@@ -2309,6 +2819,18 @@
       </c>
     </row>
     <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>70</v>
+      </c>
+      <c r="B92" t="s">
+        <v>59</v>
+      </c>
+      <c r="C92" t="s">
+        <v>26</v>
+      </c>
+      <c r="D92" t="s">
+        <v>89</v>
+      </c>
       <c r="E92" s="19">
         <f>D92-D91</f>
         <v/>
@@ -2319,6 +2841,18 @@
       </c>
     </row>
     <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>70</v>
+      </c>
+      <c r="B93" t="s">
+        <v>59</v>
+      </c>
+      <c r="C93" t="s">
+        <v>26</v>
+      </c>
+      <c r="D93" t="s">
+        <v>90</v>
+      </c>
       <c r="E93" s="19">
         <f>D93-D92</f>
         <v/>
@@ -2329,6 +2863,18 @@
       </c>
     </row>
     <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>70</v>
+      </c>
+      <c r="B94" t="s">
+        <v>59</v>
+      </c>
+      <c r="C94" t="s">
+        <v>91</v>
+      </c>
+      <c r="D94" t="s">
+        <v>78</v>
+      </c>
       <c r="E94" s="19">
         <f>D94-D93</f>
         <v/>
@@ -2339,6 +2885,18 @@
       </c>
     </row>
     <row r="95" spans="1:8">
+      <c r="A95" t="s">
+        <v>70</v>
+      </c>
+      <c r="B95" t="s">
+        <v>59</v>
+      </c>
+      <c r="C95" t="s">
+        <v>91</v>
+      </c>
+      <c r="D95" t="s">
+        <v>92</v>
+      </c>
       <c r="E95" s="19">
         <f>D95-D94</f>
         <v/>
@@ -2349,6 +2907,18 @@
       </c>
     </row>
     <row r="96" spans="1:8">
+      <c r="A96" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" t="s">
+        <v>26</v>
+      </c>
+      <c r="D96" t="s">
+        <v>71</v>
+      </c>
       <c r="E96" s="19">
         <f>D96-D95</f>
         <v/>
@@ -2359,6 +2929,18 @@
       </c>
     </row>
     <row r="97" spans="1:8">
+      <c r="A97" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" t="s">
+        <v>93</v>
+      </c>
       <c r="E97" s="19">
         <f>D97-D96</f>
         <v/>
@@ -2369,6 +2951,18 @@
       </c>
     </row>
     <row r="98" spans="1:8">
+      <c r="A98" t="s">
+        <v>94</v>
+      </c>
+      <c r="B98" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" t="s">
+        <v>74</v>
+      </c>
       <c r="E98" s="19">
         <f>D98-D97</f>
         <v/>
@@ -2379,6 +2973,18 @@
       </c>
     </row>
     <row r="99" spans="1:8">
+      <c r="A99" t="s">
+        <v>94</v>
+      </c>
+      <c r="B99" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" t="s">
+        <v>95</v>
+      </c>
       <c r="E99" s="19">
         <f>D99-D98</f>
         <v/>
@@ -2389,6 +2995,18 @@
       </c>
     </row>
     <row r="100" spans="1:8">
+      <c r="A100" t="s">
+        <v>94</v>
+      </c>
+      <c r="B100" t="s">
+        <v>59</v>
+      </c>
+      <c r="C100" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" t="s">
+        <v>96</v>
+      </c>
       <c r="E100" s="19">
         <f>D100-D99</f>
         <v/>
@@ -2399,6 +3017,18 @@
       </c>
     </row>
     <row r="101" spans="1:8">
+      <c r="A101" t="s">
+        <v>94</v>
+      </c>
+      <c r="B101" t="s">
+        <v>59</v>
+      </c>
+      <c r="C101" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" t="s">
+        <v>97</v>
+      </c>
       <c r="E101" s="19">
         <f>D101-D100</f>
         <v/>
@@ -2409,6 +3039,18 @@
       </c>
     </row>
     <row r="102" spans="1:8">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+      <c r="B102" t="s">
+        <v>59</v>
+      </c>
+      <c r="C102" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" t="s">
+        <v>98</v>
+      </c>
       <c r="E102" s="19">
         <f>D102-D101</f>
         <v/>
@@ -2419,6 +3061,18 @@
       </c>
     </row>
     <row r="103" spans="1:8">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" t="s">
+        <v>59</v>
+      </c>
+      <c r="C103" t="s">
+        <v>26</v>
+      </c>
+      <c r="D103" t="s">
+        <v>99</v>
+      </c>
       <c r="E103" s="19">
         <f>D103-D102</f>
         <v/>
@@ -2429,6 +3083,9 @@
       </c>
     </row>
     <row r="104" spans="1:8">
+      <c r="A104" t="s">
+        <v>100</v>
+      </c>
       <c r="E104" s="19">
         <f>D104-D103</f>
         <v/>

</xml_diff>

<commit_message>
working with list of equipment
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80000571.xlsx
+++ b/eq_log/eq_file/80000571.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>244</t>
+  </si>
+  <si>
+    <t>245</t>
   </si>
   <si>
     <t>**</t>
@@ -3084,6 +3087,15 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
+        <v>94</v>
+      </c>
+      <c r="B104" t="s">
+        <v>59</v>
+      </c>
+      <c r="C104" t="s">
+        <v>91</v>
+      </c>
+      <c r="D104" t="s">
         <v>100</v>
       </c>
       <c r="E104" s="19">
@@ -3096,6 +3108,9 @@
       </c>
     </row>
     <row r="105" spans="1:8">
+      <c r="A105" t="s">
+        <v>101</v>
+      </c>
       <c r="E105" s="19">
         <f>D105-D104</f>
         <v/>

</xml_diff>

<commit_message>
add list of equipment
</commit_message>
<xml_diff>
--- a/eq_log/eq_file/80000571.xlsx
+++ b/eq_log/eq_file/80000571.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
   <si>
     <t>тип обладнання</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>245</t>
+  </si>
+  <si>
+    <t>246</t>
   </si>
   <si>
     <t>**</t>
@@ -3109,6 +3112,15 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
+        <v>94</v>
+      </c>
+      <c r="B105" t="s">
+        <v>59</v>
+      </c>
+      <c r="C105" t="s">
+        <v>91</v>
+      </c>
+      <c r="D105" t="s">
         <v>101</v>
       </c>
       <c r="E105" s="19">
@@ -3121,6 +3133,9 @@
       </c>
     </row>
     <row r="106" spans="1:8">
+      <c r="A106" t="s">
+        <v>102</v>
+      </c>
       <c r="E106" s="19">
         <f>D106-D105</f>
         <v/>

</xml_diff>